<commit_message>
added new method and code refactor
</commit_message>
<xml_diff>
--- a/test_data/test_data.xlsx
+++ b/test_data/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joyde\projs\RoboApiTest\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB035E11-EBC5-4676-8562-9D137A648C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E8E0DE-02B4-4A12-84C0-D7C215CABF9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5EF8873B-B5AE-49D8-BE0C-DCAD90485ED4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>*** Test Cases ***</t>
   </si>
@@ -62,9 +62,6 @@
     <t>SINGLE &lt;RESOURCE&gt; NOT FOUND</t>
   </si>
   <si>
-    <t>${params}</t>
-  </si>
-  <si>
     <t>${resp_code}</t>
   </si>
   <si>
@@ -86,12 +83,6 @@
     <t>GET</t>
   </si>
   <si>
-    <t>${failure_tag}</t>
-  </si>
-  <si>
-    <t>page=2,per_page=6</t>
-  </si>
-  <si>
     <t>users/2</t>
   </si>
   <si>
@@ -105,6 +96,62 @@
   </si>
   <si>
     <t>unknown/23</t>
+  </si>
+  <si>
+    <t>['page']=2
+['per_page']=6
+['ad']['company']=StatusCode Weekly</t>
+  </si>
+  <si>
+    <t>CREATE</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>${req_body}</t>
+  </si>
+  <si>
+    <t>${debug_flag}</t>
+  </si>
+  <si>
+    <t>{
+"name": "morpheus",
+"job": "leader"
+}</t>
+  </si>
+  <si>
+    <t>${query_params}</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>{
+"name": "morpheus",
+"job": "zion resident2"
+}</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>UPDATE PATCH</t>
+  </si>
+  <si>
+    <t>UPDATE PUT</t>
+  </si>
+  <si>
+    <t>regression, smoke</t>
+  </si>
+  <si>
+    <t>Testing post method</t>
   </si>
 </sst>
 </file>
@@ -120,8 +167,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FF24292E"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -135,7 +183,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,24 +197,24 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFDFE2E5"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFDFE2E5"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFDFE2E5"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFDFE2E5"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -176,23 +224,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,158 +591,276 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84729F4B-418B-44F1-9946-DC7248A3E290}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" style="15" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="7">
+        <v>200</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="7">
+        <v>200</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D4" s="7">
+        <v>404</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7">
+        <v>200</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7">
+        <v>200</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="7">
+        <v>404</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="9">
+        <v>201</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2">
+      <c r="D9" s="9">
         <v>200</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="E9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="D10" s="9">
         <v>200</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="E10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="4">
-        <v>404</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7">
-        <v>404</v>
-      </c>
+      <c r="D11" s="9">
+        <v>204</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -683,12 +870,181 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF023EE2-24FA-400B-8878-D44A9CF549AB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1">
+        <v>200</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3">
+        <v>404</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>404</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1">
+        <v>201</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1">
+        <v>200</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>